<commit_message>
Added Machine Learning Model
</commit_message>
<xml_diff>
--- a/your-project/Experiment Details/Sample Details.xlsx
+++ b/your-project/Experiment Details/Sample Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccaestiarte/Desktop/IronHack/PROJECTS/Project-Week-8-Final-Project/your-project/Experiment Details/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE56467C-5BB0-FF49-AFAE-53AA55D435B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1E5D96-82A8-2E4A-ACF2-92233459DB95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="2900" windowWidth="27640" windowHeight="16940" xr2:uid="{F33C1B74-3B43-814C-B702-B9EC64D05BA0}"/>
   </bookViews>
@@ -615,7 +615,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>